<commit_message>
Revert "Revert "Report generator""
This reverts commit c6a44974b66071fb0504ab56659b86a39e651ed1.
</commit_message>
<xml_diff>
--- a/Source/Amba.Report.Test/Amba.Report.Test/Templates/Orders3.xlsx
+++ b/Source/Amba.Report.Test/Amba.Report.Test/Templates/Orders3.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="36210" yWindow="120" windowWidth="23775" windowHeight="15015"/>
+    <workbookView xWindow="39930" yWindow="120" windowWidth="23775" windowHeight="15015"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="3" r:id="rId1"/>
+    <sheet name="Page2" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Categories">Orders!$7:$7,Orders!$11:$11</definedName>
+    <definedName name="Categories">Orders!$7:$7,Orders!$11:$11,Page2!$7:$7,Orders!$13:$13</definedName>
     <definedName name="Categories.Amount">Orders!$E$11</definedName>
-    <definedName name="Categories.Name">Orders!$A$7</definedName>
-    <definedName name="Categories.Products">Orders!$8:$8,Orders!$10:$10</definedName>
+    <definedName name="Categories.Name">Orders!$A$7,Orders!$A$13</definedName>
+    <definedName name="Categories.Products">Orders!$10:$10,Orders!$8:$8</definedName>
     <definedName name="Categories.Products.Amount">Orders!$E$10</definedName>
     <definedName name="Categories.Products.Name">Orders!$A$8</definedName>
     <definedName name="Categories.Products.Orders">Orders!$9:$9</definedName>
@@ -26,10 +27,10 @@
     <definedName name="Categories.Products.Orders.Qnt">Orders!$D$9</definedName>
     <definedName name="Categories.Products.Qnt">Orders!$D$10</definedName>
     <definedName name="Categories.Qnt">Orders!$D$11</definedName>
-    <definedName name="Company.Address">Orders!$B$4</definedName>
-    <definedName name="Company.Name">Orders!$B$3</definedName>
-    <definedName name="Date">Orders!$B$2</definedName>
-    <definedName name="PrintedAt">Orders!$B$13</definedName>
+    <definedName name="Company.Address">Orders!$B$4,Page2!$B$4</definedName>
+    <definedName name="Company.Name">Orders!$B$3,Page2!$B$3</definedName>
+    <definedName name="Date">Orders!$B$2,Page2!$B$2</definedName>
+    <definedName name="PrintedAt">Orders!$B$15,Page2!$B$13</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <webPublishing codePage="1252"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Amount</t>
   </si>
@@ -78,7 +79,7 @@
     <t>Company: {Company.Name}</t>
   </si>
   <si>
-    <t>Report date: {Date: MMM dd, yyyy}</t>
+    <t>Report date: {Date:dd.MM.yyyy}</t>
   </si>
 </sst>
 </file>
@@ -223,6 +224,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -256,7 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -603,16 +604,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="3" width="14" customWidth="1"/>
-    <col min="4" max="5" width="10.75" style="3" customWidth="1"/>
+    <col min="4" max="5" width="11" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15">
@@ -634,11 +635,11 @@
       <c r="B4" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -647,29 +648,29 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="6">
         <v>0</v>
       </c>
@@ -678,11 +679,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="7">
         <v>0</v>
       </c>
@@ -691,11 +692,155 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="3" width="14" customWidth="1"/>
+    <col min="4" max="5" width="11" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="A7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="8">
         <v>0</v>
       </c>
@@ -707,8 +852,8 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -716,7 +861,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -726,11 +871,10 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix printing on several pages
</commit_message>
<xml_diff>
--- a/Source/Amba.Report.Test/Amba.Report.Test/Templates/Orders3.xlsx
+++ b/Source/Amba.Report.Test/Amba.Report.Test/Templates/Orders3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39930" yWindow="120" windowWidth="23775" windowHeight="15015"/>
+    <workbookView xWindow="41055" yWindow="120" windowWidth="23775" windowHeight="15015"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Categories">Orders!$7:$7,Orders!$11:$11,Page2!$7:$7,Orders!$13:$13</definedName>
     <definedName name="Categories.Amount">Orders!$E$11</definedName>
-    <definedName name="Categories.Name">Orders!$A$7,Orders!$A$13</definedName>
+    <definedName name="Categories.Name">Orders!$A$7,Orders!$A$13,Page2!$A$7</definedName>
     <definedName name="Categories.Products">Orders!$10:$10,Orders!$8:$8</definedName>
     <definedName name="Categories.Products.Amount">Orders!$E$10</definedName>
     <definedName name="Categories.Products.Name">Orders!$A$8</definedName>
@@ -607,7 +607,7 @@
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -751,7 +751,7 @@
   <dimension ref="A2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E7"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>